<commit_message>
fix file & boot
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miltontulli/Documents/proyectos/tincho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10C4232-B12F-724F-97EE-AC65AEBA02C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1A3662-390D-244C-91D1-3FD9F20DBCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="304">
   <si>
     <t>Shipment Number:</t>
   </si>
@@ -5534,1603 +5534,1142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0EC74E-EF54-446F-9470-8966E0CF0071}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="20" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7" style="22" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:8" ht="16">
       <c r="A1" s="18" t="s">
-        <v>303</v>
+        <v>138</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>140</v>
       </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="H1" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="20" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:8">
       <c r="A2" s="24" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24" t="str">
-        <f>_xlfn.CONCAT(B2," ",H2)</f>
-        <v>1349G NAVY 10 144</v>
-      </c>
-      <c r="E2" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="25">
+        <v>10</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26">
+        <v>144</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="24">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="B3" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G2" s="25">
+      <c r="C3" s="27">
+        <v>12</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="9">
+        <v>96</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="27">
+        <v>14</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="9">
+        <v>96</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="27">
+        <v>16</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="9">
+        <v>48</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="27">
+        <v>18</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="9">
+        <v>48</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="27">
+        <v>20</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="9">
+        <v>48</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="9">
+        <v>48</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="27">
+        <v>4</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="9">
+        <v>48</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H9" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="9">
+        <v>48</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H10" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="27">
+        <v>5</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="9">
+        <v>96</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H11" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="27">
+        <v>6</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="9">
+        <v>96</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H12" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="9">
+        <v>48</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="27">
+        <v>7</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="9">
+        <v>96</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H14" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15">
+      <c r="A15" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="32">
+        <v>8</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="9">
+        <v>192</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H15" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="A16" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="40">
+        <v>10.5</v>
+      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41">
+        <v>48</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="H16" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15">
+      <c r="A17" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="40">
+        <v>14.5</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41">
+        <v>432</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="H17" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15">
+      <c r="A18" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="40">
         <v>10</v>
       </c>
-      <c r="H2" s="26">
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41">
+        <v>384</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="H18" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15">
+      <c r="A19" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="40">
+        <v>14</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41">
+        <v>720</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>228</v>
+      </c>
+      <c r="H19" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15">
+      <c r="A20" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="40">
+        <v>16</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41">
+        <v>672</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="H20" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15">
+      <c r="A21" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="40">
+        <v>18</v>
+      </c>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41">
+        <v>432</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="H21" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15">
+      <c r="A22" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="40">
+        <v>20</v>
+      </c>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41">
+        <v>384</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="H22" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15">
+      <c r="A23" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41">
+        <v>288</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="H23" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15">
+      <c r="A24" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41">
+        <v>528</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="H24" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15">
+      <c r="A25" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="40">
+        <v>5</v>
+      </c>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="41">
         <v>144</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="G25" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="H25" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15">
+      <c r="A26" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="40">
+        <v>8</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="41">
+        <v>672</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="H26" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15">
+      <c r="A27" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="40">
+        <v>10</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="41">
+        <v>144</v>
+      </c>
+      <c r="G27" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="J2" s="24">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="24" t="str">
-        <f t="shared" ref="D3:D51" si="0">_xlfn.CONCAT(B3," ",H3)</f>
-        <v>1349G NAVY 12 96</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="H27" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15">
+      <c r="A28" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="40">
+        <v>12</v>
+      </c>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="41">
+        <v>1920</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="H28" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15">
+      <c r="A29" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" s="40">
+        <v>14</v>
+      </c>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41">
+        <v>480</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>228</v>
+      </c>
+      <c r="H29" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15">
+      <c r="A30" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="40">
+        <v>16</v>
+      </c>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="41">
+        <v>768</v>
+      </c>
+      <c r="G30" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="H30" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15">
+      <c r="A31" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="40">
+        <v>18</v>
+      </c>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="41">
+        <v>768</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="H31" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15">
+      <c r="A32" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="40">
+        <v>20</v>
+      </c>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="41">
+        <v>720</v>
+      </c>
+      <c r="G32" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="H32" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15">
+      <c r="A33" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="41">
+        <v>96</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="H33" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15">
+      <c r="A34" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="41">
+        <v>384</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="H34" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15">
+      <c r="A35" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41">
+        <v>672</v>
+      </c>
+      <c r="G35" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="H35" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15">
+      <c r="A36" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="40">
+        <v>6</v>
+      </c>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="41">
+        <v>1056</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="H36" s="36">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G3" s="27">
+      <c r="C37" s="27">
+        <v>18</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="9">
+        <v>48</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="H37" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="27">
+        <v>10</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="9">
+        <v>48</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="H38" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="27">
         <v>12</v>
       </c>
-      <c r="H3" s="9">
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="9">
+        <v>48</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="H39" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" s="27">
+        <v>14</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="9">
         <v>96</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="J3" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349G NAVY 14 96</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="G40" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="H40" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="27">
+        <v>18</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="9">
+        <v>48</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="H41" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="27">
+        <v>20</v>
+      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="9">
+        <v>48</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="H42" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="27">
-        <v>14</v>
-      </c>
-      <c r="H4" s="9">
-        <v>96</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="J4" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349N NAVY 16 48</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="F5" s="13" t="s">
+      <c r="C43" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="9">
+        <v>48</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="H43" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="27">
-        <v>16</v>
-      </c>
-      <c r="H5" s="9">
-        <v>48</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="J5" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349N NAVY 18 48</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="F6" s="13" t="s">
+      <c r="C44" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="9">
+        <v>48</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="H44" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="9">
+        <v>48</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="H45" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="9">
+        <v>48</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="H46" s="13">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15">
+      <c r="A47" s="29">
+        <v>16996</v>
+      </c>
+      <c r="B47" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="G6" s="27">
-        <v>18</v>
-      </c>
-      <c r="H6" s="9">
-        <v>48</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="J6" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349N NAVY 20 48</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G7" s="27">
-        <v>20</v>
-      </c>
-      <c r="H7" s="9">
-        <v>48</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J7" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349Q NAVY 3T 48</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="9">
-        <v>48</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="J8" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349B NAVY 4 48</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G9" s="27">
-        <v>4</v>
-      </c>
-      <c r="H9" s="9">
-        <v>48</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="J9" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349Q NAVY 4T 48</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="H10" s="9">
-        <v>48</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="J10" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349B NAVY 5 96</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G11" s="27">
-        <v>5</v>
-      </c>
-      <c r="H11" s="9">
-        <v>96</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="J11" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349B NAVY 6 96</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" s="27">
-        <v>6</v>
-      </c>
-      <c r="H12" s="9">
-        <v>96</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="J12" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349B NAVY 6X 48</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="H13" s="9">
-        <v>48</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="J13" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349G NAVY 7 96</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G14" s="27">
-        <v>7</v>
-      </c>
-      <c r="H14" s="9">
-        <v>96</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="J14" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1349G NAVY 8 192</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="G15" s="32">
-        <v>8</v>
-      </c>
-      <c r="H15" s="9">
-        <v>192</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="J15" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396U NAVY 10.5 48</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>297</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G16" s="40">
-        <v>10.5</v>
-      </c>
-      <c r="H16" s="41">
-        <v>48</v>
-      </c>
-      <c r="I16" s="41" t="s">
-        <v>222</v>
-      </c>
-      <c r="J16" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15">
-      <c r="A17" s="36" t="s">
-        <v>223</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396U KHAK 14.5 432</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>297</v>
-      </c>
-      <c r="F17" s="36" t="s">
+      <c r="C47" s="32">
+        <v>38</v>
+      </c>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33">
+        <v>24</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="H47" s="29">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15">
+      <c r="A48" s="29">
+        <v>16996</v>
+      </c>
+      <c r="B48" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="G17" s="40">
-        <v>14.5</v>
-      </c>
-      <c r="H17" s="41">
-        <v>432</v>
-      </c>
-      <c r="I17" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="J17" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15">
-      <c r="A18" s="36" t="s">
-        <v>224</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396G NAVY 10 384</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18" s="40">
-        <v>10</v>
-      </c>
-      <c r="H18" s="41">
-        <v>384</v>
-      </c>
-      <c r="I18" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="J18" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396G NAVY 14 720</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G19" s="40">
-        <v>14</v>
-      </c>
-      <c r="H19" s="41">
-        <v>720</v>
-      </c>
-      <c r="I19" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="J19" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15">
-      <c r="A20" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396N NAVY 16 672</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" s="40">
-        <v>16</v>
-      </c>
-      <c r="H20" s="41">
-        <v>672</v>
-      </c>
-      <c r="I20" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="J20" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="36" t="s">
-        <v>231</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396N NAVY 18 432</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G21" s="40">
-        <v>18</v>
-      </c>
-      <c r="H21" s="41">
-        <v>432</v>
-      </c>
-      <c r="I21" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="J21" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396N NAVY 20 384</v>
-      </c>
-      <c r="E22" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="40">
-        <v>20</v>
-      </c>
-      <c r="H22" s="41">
-        <v>384</v>
-      </c>
-      <c r="I22" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="J22" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396Q NAVY 2T 288</v>
-      </c>
-      <c r="E23" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="H23" s="41">
-        <v>288</v>
-      </c>
-      <c r="I23" s="41" t="s">
-        <v>237</v>
-      </c>
-      <c r="J23" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="36" t="s">
-        <v>238</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>239</v>
-      </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396Q NAVY 3T 528</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G24" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="H24" s="41">
-        <v>528</v>
-      </c>
-      <c r="I24" s="41" t="s">
-        <v>240</v>
-      </c>
-      <c r="J24" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396B NAVY 5 144</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G25" s="40">
-        <v>5</v>
-      </c>
-      <c r="H25" s="41">
-        <v>144</v>
-      </c>
-      <c r="I25" s="41" t="s">
-        <v>243</v>
-      </c>
-      <c r="J25" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="36" t="s">
-        <v>244</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>245</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396G NAVY 8 672</v>
-      </c>
-      <c r="E26" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G26" s="40">
-        <v>8</v>
-      </c>
-      <c r="H26" s="41">
-        <v>672</v>
-      </c>
-      <c r="I26" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="J26" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="B27" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396G KHAK 10 144</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="F27" s="36" t="s">
+      <c r="C48" s="32">
+        <v>28</v>
+      </c>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="33">
+        <v>24</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="H48" s="29">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15">
+      <c r="A49" s="29">
+        <v>16996</v>
+      </c>
+      <c r="B49" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="G27" s="40">
-        <v>10</v>
-      </c>
-      <c r="H27" s="41">
-        <v>144</v>
-      </c>
-      <c r="I27" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="J27" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396G KHAK 12 1920</v>
-      </c>
-      <c r="E28" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="F28" s="36" t="s">
+      <c r="C49" s="32">
+        <v>30</v>
+      </c>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33">
+        <v>24</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="H49" s="29">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15">
+      <c r="A50" s="29">
+        <v>16996</v>
+      </c>
+      <c r="B50" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="G28" s="40">
-        <v>12</v>
-      </c>
-      <c r="H28" s="41">
-        <v>1920</v>
-      </c>
-      <c r="I28" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="J28" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="36" t="s">
-        <v>250</v>
-      </c>
-      <c r="B29" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396G KHAK 14 480</v>
-      </c>
-      <c r="E29" s="36" t="s">
-        <v>298</v>
-      </c>
-      <c r="F29" s="36" t="s">
+      <c r="C50" s="32">
+        <v>36</v>
+      </c>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="33">
+        <v>24</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="H50" s="29">
+        <v>490013265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15">
+      <c r="A51" s="29">
+        <v>16996</v>
+      </c>
+      <c r="B51" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="G29" s="40">
-        <v>14</v>
-      </c>
-      <c r="H29" s="41">
-        <v>480</v>
-      </c>
-      <c r="I29" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="J29" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="36" t="s">
-        <v>252</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396N KHAK 16 768</v>
-      </c>
-      <c r="E30" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="G30" s="40">
-        <v>16</v>
-      </c>
-      <c r="H30" s="41">
-        <v>768</v>
-      </c>
-      <c r="I30" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="J30" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="36" t="s">
-        <v>254</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>255</v>
-      </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396N KHAK 18 768</v>
-      </c>
-      <c r="E31" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="F31" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" s="40">
-        <v>18</v>
-      </c>
-      <c r="H31" s="41">
-        <v>768</v>
-      </c>
-      <c r="I31" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="J31" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396N KHAK 20 720</v>
-      </c>
-      <c r="E32" s="36" t="s">
-        <v>299</v>
-      </c>
-      <c r="F32" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="G32" s="40">
-        <v>20</v>
-      </c>
-      <c r="H32" s="41">
-        <v>720</v>
-      </c>
-      <c r="I32" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="J32" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="36" t="s">
-        <v>258</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>259</v>
-      </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396Q KHAK 2T 96</v>
-      </c>
-      <c r="E33" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="F33" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="G33" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="H33" s="41">
-        <v>96</v>
-      </c>
-      <c r="I33" s="41" t="s">
-        <v>237</v>
-      </c>
-      <c r="J33" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="36" t="s">
-        <v>260</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396Q KHAK 3T 384</v>
-      </c>
-      <c r="E34" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="G34" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="H34" s="41">
-        <v>384</v>
-      </c>
-      <c r="I34" s="41" t="s">
-        <v>240</v>
-      </c>
-      <c r="J34" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="B35" s="36" t="s">
-        <v>263</v>
-      </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396Q KHAK 4T 672</v>
-      </c>
-      <c r="E35" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="F35" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="G35" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="H35" s="41">
-        <v>672</v>
-      </c>
-      <c r="I35" s="41" t="s">
-        <v>264</v>
-      </c>
-      <c r="J35" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="36" t="s">
-        <v>265</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1396B KHAK 6 1056</v>
-      </c>
-      <c r="E36" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="F36" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="G36" s="40">
-        <v>6</v>
-      </c>
-      <c r="H36" s="41">
-        <v>1056</v>
-      </c>
-      <c r="I36" s="41" t="s">
-        <v>267</v>
-      </c>
-      <c r="J36" s="36">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699L NAVY 18 48</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G37" s="27">
-        <v>18</v>
-      </c>
-      <c r="H37" s="9">
-        <v>48</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="J37" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699F KHAK 10 48</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G38" s="27">
-        <v>10</v>
-      </c>
-      <c r="H38" s="9">
-        <v>48</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="J38" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699F KHAK 12 48</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G39" s="27">
-        <v>12</v>
-      </c>
-      <c r="H39" s="9">
-        <v>48</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="J39" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699F KHAK 14 96</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G40" s="27">
-        <v>14</v>
-      </c>
-      <c r="H40" s="9">
-        <v>96</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="J40" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699L KHAK 18 48</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="27">
-        <v>18</v>
-      </c>
-      <c r="H41" s="9">
-        <v>48</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="J41" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699L KHAK 20 48</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G42" s="27">
-        <v>20</v>
-      </c>
-      <c r="H42" s="9">
-        <v>48</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="J42" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699S NAVY 16H 48</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G43" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="H43" s="9">
-        <v>48</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="J43" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699S NAVY 20H 48</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="H44" s="9">
-        <v>48</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="J44" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699S KHAK 14H 48</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="H45" s="9">
-        <v>48</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="J45" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1699S KHAK 18H 48</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G46" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="H46" s="9">
-        <v>48</v>
-      </c>
-      <c r="I46" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="J46" s="13">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15">
-      <c r="A47" s="29" t="s">
-        <v>288</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>16996 NAVY 38 24</v>
-      </c>
-      <c r="E47" s="29">
-        <v>16996</v>
-      </c>
-      <c r="F47" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="G47" s="32">
-        <v>38</v>
-      </c>
-      <c r="H47" s="33">
+      <c r="C51" s="32">
+        <v>40</v>
+      </c>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="33">
         <v>24</v>
       </c>
-      <c r="I47" s="33" t="s">
-        <v>289</v>
-      </c>
-      <c r="J47" s="29">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15">
-      <c r="A48" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>16996 KHAK 28 24</v>
-      </c>
-      <c r="E48" s="29">
-        <v>16996</v>
-      </c>
-      <c r="F48" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" s="32">
-        <v>28</v>
-      </c>
-      <c r="H48" s="33">
-        <v>24</v>
-      </c>
-      <c r="I48" s="33" t="s">
-        <v>291</v>
-      </c>
-      <c r="J48" s="29">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15">
-      <c r="A49" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>16996 KHAK 30 24</v>
-      </c>
-      <c r="E49" s="29">
-        <v>16996</v>
-      </c>
-      <c r="F49" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="G49" s="32">
-        <v>30</v>
-      </c>
-      <c r="H49" s="33">
-        <v>24</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="J49" s="29">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15">
-      <c r="A50" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>16996 KHAK 36 24</v>
-      </c>
-      <c r="E50" s="29">
-        <v>16996</v>
-      </c>
-      <c r="F50" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="G50" s="32">
-        <v>36</v>
-      </c>
-      <c r="H50" s="33">
-        <v>24</v>
-      </c>
-      <c r="I50" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="J50" s="29">
-        <v>490013265</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="15">
-      <c r="A51" s="29" t="s">
-        <v>295</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>16996 KHAK 40 24</v>
-      </c>
-      <c r="E51" s="29">
-        <v>16996</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="G51" s="32">
-        <v>40</v>
-      </c>
-      <c r="H51" s="33">
-        <v>24</v>
-      </c>
-      <c r="I51" s="33" t="s">
+      <c r="G51" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="J51" s="29">
+      <c r="H51" s="29">
         <v>490013265</v>
       </c>
     </row>

</xml_diff>